<commit_message>
+ now the software work + no touch
</commit_message>
<xml_diff>
--- a/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
+++ b/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC Load Control Panel</t>
   </si>
 </sst>
 </file>
@@ -1443,9 +1449,7 @@
         <v>17</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
+      <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
@@ -1632,35 +1636,19 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
+ work in progress + pre cube generation
</commit_message>
<xml_diff>
--- a/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
+++ b/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">DC Load Control Panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seat Control Panel</t>
   </si>
 </sst>
 </file>
@@ -1645,7 +1648,7 @@
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5"/>

</xml_diff>

<commit_message>
+ add calibration screeen
</commit_message>
<xml_diff>
--- a/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
+++ b/DC_Load_Software/TouchGFX/assets/texts/texts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr autoCompressPictures="1"/>
   <bookViews>
-    <workbookView windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="63">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -125,9 +125,6 @@
     <t xml:space="preserve">DIRECTION</t>
   </si>
   <si>
-    <t xml:space="preserve">GB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Widget Wildcard Characters</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t xml:space="preserve">Small</t>
   </si>
   <si>
-    <t xml:space="preserve">0123456789.</t>
-  </si>
-  <si>
     <t xml:space="preserve">SingleUseId1</t>
   </si>
   <si>
@@ -155,31 +149,67 @@
     <t xml:space="preserve">LTR</t>
   </si>
   <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seat Control Panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_PRESS_TOPSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toccare il crocino in alto per calibrare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_PRESS_MIDDLEDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toccare il crocino al lato per calibrare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_PRESS_BOTTOMCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toccare il crocino sotto per calibrare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_DONE_FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibrazione non riuscita premi per uscire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_DONE_SUCCESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premere per salvare ed uscire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIB_START_RELEASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rilascia per iniziare</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">DC_Load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&gt; %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC Load Control Panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seat Control Panel</t>
+    <t xml:space="preserve">0-9,A-Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,7 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -571,7 +601,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -580,86 +609,86 @@
   <cellStyles count="82">
     <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 2" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
-    <cellStyle name="Normal 14 2" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 16" xfId="9"/>
-    <cellStyle name="Normal 16 2" xfId="10"/>
-    <cellStyle name="Normal 16 3" xfId="11"/>
-    <cellStyle name="Normal 17 2" xfId="12"/>
-    <cellStyle name="Normal 17 3" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 2 4" xfId="17"/>
-    <cellStyle name="Normal 2 5" xfId="18"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 7" xfId="20"/>
-    <cellStyle name="Normal 2 8" xfId="21"/>
-    <cellStyle name="Normal 2 9" xfId="22"/>
-    <cellStyle name="Normal 22" xfId="23"/>
-    <cellStyle name="Normal 22 10" xfId="24"/>
-    <cellStyle name="Normal 22 11" xfId="25"/>
-    <cellStyle name="Normal 22 12" xfId="26"/>
-    <cellStyle name="Normal 22 13" xfId="27"/>
-    <cellStyle name="Normal 22 14" xfId="28"/>
-    <cellStyle name="Normal 22 15" xfId="29"/>
-    <cellStyle name="Normal 22 16" xfId="30"/>
-    <cellStyle name="Normal 22 17" xfId="31"/>
-    <cellStyle name="Normal 22 18" xfId="32"/>
-    <cellStyle name="Normal 22 2" xfId="33"/>
-    <cellStyle name="Normal 22 3" xfId="34"/>
-    <cellStyle name="Normal 22 4" xfId="35"/>
-    <cellStyle name="Normal 22 5" xfId="36"/>
-    <cellStyle name="Normal 22 6" xfId="37"/>
-    <cellStyle name="Normal 22 7" xfId="38"/>
-    <cellStyle name="Normal 22 8" xfId="39"/>
-    <cellStyle name="Normal 22 9" xfId="40"/>
-    <cellStyle name="Normal 23 10" xfId="41"/>
-    <cellStyle name="Normal 23 11" xfId="42"/>
-    <cellStyle name="Normal 23 12" xfId="43"/>
-    <cellStyle name="Normal 23 13" xfId="44"/>
-    <cellStyle name="Normal 23 14" xfId="45"/>
-    <cellStyle name="Normal 23 15" xfId="46"/>
-    <cellStyle name="Normal 23 16" xfId="47"/>
-    <cellStyle name="Normal 23 17" xfId="48"/>
-    <cellStyle name="Normal 23 18" xfId="49"/>
-    <cellStyle name="Normal 23 2" xfId="50"/>
-    <cellStyle name="Normal 23 3" xfId="51"/>
-    <cellStyle name="Normal 23 4" xfId="52"/>
-    <cellStyle name="Normal 23 5" xfId="53"/>
-    <cellStyle name="Normal 23 6" xfId="54"/>
-    <cellStyle name="Normal 23 7" xfId="55"/>
-    <cellStyle name="Normal 23 8" xfId="56"/>
-    <cellStyle name="Normal 23 9" xfId="57"/>
-    <cellStyle name="Normal 25 10" xfId="58"/>
-    <cellStyle name="Normal 25 11" xfId="59"/>
-    <cellStyle name="Normal 25 12" xfId="60"/>
-    <cellStyle name="Normal 25 13" xfId="61"/>
-    <cellStyle name="Normal 25 14" xfId="62"/>
-    <cellStyle name="Normal 25 15" xfId="63"/>
-    <cellStyle name="Normal 25 16" xfId="64"/>
-    <cellStyle name="Normal 25 17" xfId="65"/>
-    <cellStyle name="Normal 25 2" xfId="66"/>
-    <cellStyle name="Normal 25 3" xfId="67"/>
-    <cellStyle name="Normal 25 4" xfId="68"/>
-    <cellStyle name="Normal 25 5" xfId="69"/>
-    <cellStyle name="Normal 25 6" xfId="70"/>
-    <cellStyle name="Normal 25 7" xfId="71"/>
-    <cellStyle name="Normal 25 8" xfId="72"/>
-    <cellStyle name="Normal 25 9" xfId="73"/>
-    <cellStyle name="Normal 3" xfId="74"/>
-    <cellStyle name="Normal 4" xfId="75"/>
-    <cellStyle name="Normal 5" xfId="76"/>
-    <cellStyle name="Normal 6" xfId="77"/>
-    <cellStyle name="Normal 7" xfId="78"/>
-    <cellStyle name="Normal 8" xfId="79"/>
-    <cellStyle name="Normal 9" xfId="80"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 10 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 12" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 13" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 14" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 14 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 15" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 16" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 16 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 16 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 17 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 17 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 3" xfId="16" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2 4" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 5" xfId="18" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 6" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 2 7" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 2 8" xfId="21" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 2 9" xfId="22" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 22" xfId="23" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 22 10" xfId="24" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 22 11" xfId="25" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 22 12" xfId="26" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 22 13" xfId="27" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 22 14" xfId="28" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 22 15" xfId="29" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 22 16" xfId="30" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 22 17" xfId="31" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 22 18" xfId="32" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 22 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 22 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 22 4" xfId="35" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 22 5" xfId="36" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 22 6" xfId="37" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 22 7" xfId="38" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 22 8" xfId="39" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 22 9" xfId="40" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 23 10" xfId="41" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 23 11" xfId="42" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 23 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 23 13" xfId="44" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 23 14" xfId="45" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 23 15" xfId="46" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 23 16" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 23 17" xfId="48" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 23 18" xfId="49" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 23 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 23 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 23 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 23 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 23 6" xfId="54" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 23 7" xfId="55" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 23 8" xfId="56" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 23 9" xfId="57" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 25 10" xfId="58" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 25 11" xfId="59" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 25 12" xfId="60" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 25 13" xfId="61" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 25 14" xfId="62" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 25 15" xfId="63" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 25 16" xfId="64" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 25 17" xfId="65" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 25 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 25 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 25 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 25 5" xfId="69" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 25 6" xfId="70" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 25 7" xfId="71" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 25 8" xfId="72" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 25 9" xfId="73" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 3" xfId="74" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 4" xfId="75" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 5" xfId="76" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 6" xfId="77" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 7" xfId="78" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 8" xfId="79" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 9" xfId="80" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -899,7 +928,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="firstColumn" dxfId="15"/>
       <tableStyleElement type="lastColumn" dxfId="14"/>
@@ -921,33 +950,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
-  <sortState ref="B4:E6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:E6">
     <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Typography Name"/>
-    <tableColumn id="2" name="Font"/>
-    <tableColumn id="3" name="Size"/>
-    <tableColumn id="4" name="Bpp"/>
-    <tableColumn id="5" name="Fallback Character"/>
-    <tableColumn id="6" name="Wildcard Characters"/>
-    <tableColumn id="9" name="Widget Wildcard Characters"/>
-    <tableColumn id="7" name="Wildcard Ranges"/>
-    <tableColumn id="8" name="Ellipsis Character"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Typography Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Font"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Size"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Bpp"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Fallback Character"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Wildcard Characters"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Widget Wildcard Characters"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Wildcard Ranges"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ellipsis Character"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
-    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
-    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Example 1" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Example 2" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Example 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1358,16 +1387,16 @@
       <c r="E1"/>
     </row>
     <row r="2" spans="2:16" ht="39.95" customHeight="1" thickBot="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1">
@@ -1389,8 +1418,8 @@
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>37</v>
+      <c r="H3" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>6</v>
@@ -1401,10 +1430,10 @@
     </row>
     <row r="4" spans="2:16">
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -1417,7 +1446,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1437,10 +1468,10 @@
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -1471,10 +1502,10 @@
     </row>
     <row r="6" spans="2:16">
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1592,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F3"/>
+  <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1610,12 +1641,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="3.75" customHeight="1"/>
     <row r="2" spans="2:6" ht="33" customHeight="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:6" s="22" customFormat="1">
       <c r="B3" t="s">
@@ -1631,27 +1662,145 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5"/>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>